<commit_message>
Added house elements for basic outline to calculator
</commit_message>
<xml_diff>
--- a/HolidayCoroOutlineCalculator.xlsx
+++ b/HolidayCoroOutlineCalculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanbryant/Projects/house-lights/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DEEDF76-9ED3-B448-8E1B-07404C372F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A7BE91-C7B3-D945-B392-71D54580780F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="5" r:id="rId1"/>
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="140">
   <si>
     <t>Section Description</t>
   </si>
@@ -478,12 +478,6 @@
     <t>Square</t>
   </si>
   <si>
-    <t>Sample</t>
-  </si>
-  <si>
-    <t>Enter your data into only the green sections</t>
-  </si>
-  <si>
     <t>http://www.holidaycoro.com/product-p/673.htm</t>
   </si>
   <si>
@@ -623,6 +617,27 @@
   </si>
   <si>
     <t>Item #709-12 RGB Brilliant Bulb - Strawberry bulb (2 LED/1 IC) 12 Inch Spacing</t>
+  </si>
+  <si>
+    <t>Left Angle, Left Side</t>
+  </si>
+  <si>
+    <t>Left Angle, Right Side</t>
+  </si>
+  <si>
+    <t>Right Angle, Left Side</t>
+  </si>
+  <si>
+    <t>Right Angle, Right Side</t>
+  </si>
+  <si>
+    <t>Left Side of Garage</t>
+  </si>
+  <si>
+    <t>Top of Garage</t>
+  </si>
+  <si>
+    <t>Right Side of Garage</t>
   </si>
 </sst>
 </file>
@@ -1755,7 +1770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B5:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7:N7"/>
     </sheetView>
   </sheetViews>
@@ -1766,7 +1781,7 @@
   <sheetData>
     <row r="5" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C5" s="75"/>
       <c r="D5" s="75"/>
@@ -1783,7 +1798,7 @@
     </row>
     <row r="6" spans="2:14" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="77" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C6" s="78"/>
       <c r="D6" s="78"/>
@@ -1822,24 +1837,24 @@
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I11" s="67" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I12" s="67"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I13" s="67" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
@@ -1859,7 +1874,7 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1881,8 +1896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1905,7 +1920,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="86" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B1" s="86"/>
       <c r="C1" s="86"/>
@@ -2002,7 +2017,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="65" t="s">
-        <v>86</v>
+        <v>133</v>
       </c>
       <c r="B4" s="43">
         <v>1</v>
@@ -2020,55 +2035,55 @@
       </c>
       <c r="F4" s="21">
         <f>ROUNDUP((D4/CONVERT($B$28,"in","ft")),0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G4" s="21">
         <f>SUM(F4*3)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H4" s="23">
         <f t="shared" ref="H4:H23" si="0">SUM(F4*$I$28)</f>
-        <v>0.96</v>
+        <v>2.88</v>
       </c>
       <c r="I4" s="24">
         <f t="shared" ref="I4:I23" si="1">SUM(F4*$H$28)</f>
-        <v>1.7196</v>
+        <v>2.8311999999999999</v>
       </c>
       <c r="J4" s="25">
         <f>SUM(((H4/$E$28)*0.002525)*2)</f>
-        <v>4.0400000000000001E-4</v>
+        <v>1.212E-3</v>
       </c>
       <c r="K4" s="26">
         <f>SUM(((H4/$E$28)*0.00402)*2)</f>
-        <v>6.4320000000000002E-4</v>
+        <v>1.9296000000000001E-3</v>
       </c>
       <c r="L4" s="26">
         <f>SUM(((H4/$E$28)*0.00639)*2)</f>
-        <v>1.0223999999999999E-3</v>
+        <v>3.0672E-3</v>
       </c>
       <c r="M4" s="26">
         <f>SUM(((H4/$E$28)*0.01015)*2)</f>
-        <v>1.624E-3</v>
+        <v>4.8719999999999996E-3</v>
       </c>
       <c r="N4" s="26">
         <f>SUM(((H4/$E$28)*0.01614)*2)</f>
-        <v>2.5824000000000003E-3</v>
+        <v>7.7472000000000001E-3</v>
       </c>
       <c r="O4" s="27">
         <f>SUM(((H4/$E$28)*0.02567)*2)</f>
-        <v>4.1072000000000001E-3</v>
+        <v>1.2321599999999999E-2</v>
       </c>
       <c r="P4" s="45" t="s">
         <v>33</v>
       </c>
       <c r="Q4" s="35">
         <f>SUM(F24)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="65" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
@@ -2131,7 +2146,9 @@
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="65"/>
+      <c r="A6" s="65" t="s">
+        <v>135</v>
+      </c>
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="D6" s="21">
@@ -2187,11 +2204,13 @@
       </c>
       <c r="Q6" s="35" t="str">
         <f>CONCATENATE(ROUND(H24,0)," Watts")</f>
-        <v>1 Watts</v>
+        <v>3 Watts</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="65"/>
+      <c r="A7" s="65" t="s">
+        <v>136</v>
+      </c>
       <c r="B7" s="43"/>
       <c r="C7" s="43"/>
       <c r="D7" s="21">
@@ -2247,11 +2266,13 @@
       </c>
       <c r="Q7" s="36" t="str">
         <f>CONCATENATE(ROUND(($H$24/5),0)," @ 5VDC")</f>
-        <v>0 @ 5VDC</v>
+        <v>1 @ 5VDC</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="65"/>
+      <c r="A8" s="65" t="s">
+        <v>137</v>
+      </c>
       <c r="B8" s="43"/>
       <c r="C8" s="43"/>
       <c r="D8" s="21">
@@ -2311,7 +2332,9 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="65"/>
+      <c r="A9" s="65" t="s">
+        <v>138</v>
+      </c>
       <c r="B9" s="43"/>
       <c r="C9" s="43"/>
       <c r="D9" s="21">
@@ -2367,11 +2390,13 @@
       </c>
       <c r="Q9" s="35">
         <f>SUM(G24)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="65"/>
+      <c r="A10" s="65" t="s">
+        <v>139</v>
+      </c>
       <c r="B10" s="43"/>
       <c r="C10" s="43"/>
       <c r="D10" s="21">
@@ -3138,19 +3163,19 @@
       </c>
       <c r="F24" s="49">
         <f>SUM(F4:F23)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G24" s="49">
         <f>SUM(G4:G23)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H24" s="51">
         <f>SUM(H4:H23)</f>
-        <v>0.96</v>
+        <v>2.88</v>
       </c>
       <c r="I24" s="52">
         <f>SUM(I4:I23)</f>
-        <v>1.7196</v>
+        <v>2.8311999999999999</v>
       </c>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
@@ -3218,11 +3243,11 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="61" t="s">
-        <v>132</v>
+        <v>98</v>
       </c>
       <c r="B28" s="38">
         <f>IF($A$28="","",INDEX('Pixel Data'!B$3:B$54,MATCH($A$28,'Pixel Data'!$A$3:$A$54,0)))</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C28" s="38">
         <f>IF($A$28="","",INDEX('Pixel Data'!C$3:C$54,MATCH($A$28,'Pixel Data'!$A$3:$A$54,0)))</f>
@@ -3230,7 +3255,7 @@
       </c>
       <c r="D28" s="39">
         <f>IF($A$28="","",INDEX('Pixel Data'!D$3:D$54,MATCH($A$28,'Pixel Data'!$A$3:$A$54,0)))</f>
-        <v>42.99</v>
+        <v>35.39</v>
       </c>
       <c r="E28" s="38">
         <f>IF($A$28="","",INDEX('Pixel Data'!E$3:E$54,MATCH($A$28,'Pixel Data'!$A$3:$A$54,0)))</f>
@@ -3238,23 +3263,23 @@
       </c>
       <c r="F28" s="38">
         <f>IF($A$28="","",INDEX('Pixel Data'!F$3:F$54,MATCH($A$28,'Pixel Data'!$A$3:$A$54,0)))</f>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="G28" s="38" t="str">
         <f>IF($A$28="","",INDEX('Pixel Data'!G$3:G$54,MATCH($A$28,'Pixel Data'!$A$3:$A$54,0)))</f>
-        <v>8 Inch Spacing</v>
+        <v>30 LED / 10 IC</v>
       </c>
       <c r="H28" s="39">
         <f>IF($A$28="","",INDEX('Pixel Data'!H$3:H$54,MATCH($A$28,'Pixel Data'!$A$3:$A$54,0)))</f>
-        <v>0.85980000000000001</v>
+        <v>0.70779999999999998</v>
       </c>
       <c r="I28" s="38">
         <f>IF($A$28="","",INDEX('Pixel Data'!I$3:I$54,MATCH($A$28,'Pixel Data'!$A$3:$A$54,0)))</f>
-        <v>0.48</v>
+        <v>0.72</v>
       </c>
       <c r="J28" s="38">
         <f>IF($A$28="","",INDEX('Pixel Data'!J$3:J$54,MATCH($A$28,'Pixel Data'!$A$3:$A$54,0)))</f>
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="K28" s="38">
         <f>IF($A$28="","",INDEX('Pixel Data'!K$3:K$54,MATCH($A$28,'Pixel Data'!$A$3:$A$54,0)))</f>
@@ -3395,7 +3420,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="72" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B3" s="20">
         <v>4</v>
@@ -3444,7 +3469,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="72" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" s="20">
         <v>2.44</v>
@@ -3493,7 +3518,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="72" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B5" s="20">
         <v>1.97</v>
@@ -3542,7 +3567,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="72" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B6" s="20">
         <v>4</v>
@@ -3560,7 +3585,7 @@
         <v>60</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H6" s="55">
         <f t="shared" si="0"/>
@@ -3583,7 +3608,7 @@
         <v>150</v>
       </c>
       <c r="M6" s="64" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
@@ -3591,7 +3616,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="72" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B7" s="20">
         <v>0.65</v>
@@ -3609,7 +3634,7 @@
         <v>60</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H7" s="55">
         <f t="shared" si="0"/>
@@ -3632,7 +3657,7 @@
         <v>300</v>
       </c>
       <c r="M7" s="64" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
@@ -3640,7 +3665,7 @@
     </row>
     <row r="8" spans="1:16" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="72" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B8" s="20">
         <v>8</v>
@@ -3658,7 +3683,7 @@
         <v>40</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H8" s="55">
         <f t="shared" si="0"/>
@@ -3681,7 +3706,7 @@
         <v>50</v>
       </c>
       <c r="M8" s="64" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
@@ -3689,7 +3714,7 @@
     </row>
     <row r="9" spans="1:16" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="72" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B9" s="20">
         <v>10</v>
@@ -3707,7 +3732,7 @@
         <v>40</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H9" s="55">
         <f t="shared" si="0"/>
@@ -3730,7 +3755,7 @@
         <v>50</v>
       </c>
       <c r="M9" s="64" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
@@ -3738,7 +3763,7 @@
     </row>
     <row r="10" spans="1:16" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="72" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B10" s="20">
         <v>12</v>
@@ -3756,7 +3781,7 @@
         <v>40</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H10" s="55">
         <f t="shared" si="0"/>
@@ -3779,7 +3804,7 @@
         <v>50</v>
       </c>
       <c r="M10" s="64" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
@@ -3787,7 +3812,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="71" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B11" s="20">
         <v>1</v>
@@ -3835,7 +3860,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="71" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B12" s="20">
         <v>2</v>
@@ -3883,7 +3908,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="71" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B13" s="20">
         <v>3</v>
@@ -3931,7 +3956,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="72" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B14" s="20">
         <v>4</v>
@@ -3971,7 +3996,7 @@
         <v>1</v>
       </c>
       <c r="M14" s="64" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
@@ -3979,7 +4004,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="72" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B15" s="20">
         <v>5</v>
@@ -4019,7 +4044,7 @@
         <v>1</v>
       </c>
       <c r="M15" s="64" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
@@ -4027,7 +4052,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="72" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B16" s="20">
         <v>6</v>
@@ -4067,7 +4092,7 @@
         <v>1</v>
       </c>
       <c r="M16" s="64" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
@@ -4075,7 +4100,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="71" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B17" s="20">
         <v>1</v>
@@ -4115,7 +4140,7 @@
         <v>1</v>
       </c>
       <c r="M17" s="64" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
@@ -4123,7 +4148,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="71" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B18" s="20">
         <v>2</v>
@@ -4163,7 +4188,7 @@
         <v>1</v>
       </c>
       <c r="M18" s="64" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
@@ -4171,7 +4196,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="71" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B19" s="20">
         <v>3</v>
@@ -4211,7 +4236,7 @@
         <v>1</v>
       </c>
       <c r="M19" s="64" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
@@ -4219,7 +4244,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="72" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B20" s="20">
         <v>1</v>
@@ -4268,7 +4293,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="72" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B21" s="20">
         <v>2</v>
@@ -4317,7 +4342,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="72" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B22" s="20">
         <v>3</v>
@@ -4366,7 +4391,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="71" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B23" s="20">
         <v>1</v>
@@ -4407,7 +4432,7 @@
         <v>1</v>
       </c>
       <c r="M23" s="64" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
@@ -4415,7 +4440,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="71" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B24" s="20">
         <v>2</v>
@@ -4456,7 +4481,7 @@
         <v>1</v>
       </c>
       <c r="M24" s="64" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
@@ -4464,7 +4489,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="71" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B25" s="20">
         <v>3</v>
@@ -4505,7 +4530,7 @@
         <v>1</v>
       </c>
       <c r="M25" s="64" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
@@ -4513,7 +4538,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="71" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B26" s="20">
         <v>3</v>
@@ -4554,7 +4579,7 @@
         <v>1</v>
       </c>
       <c r="M26" s="64" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
@@ -4562,7 +4587,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="71" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B27" s="20">
         <v>3</v>
@@ -4603,7 +4628,7 @@
         <v>1</v>
       </c>
       <c r="M27" s="64" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>

</xml_diff>

<commit_message>
Update calculator spreadsheet and outline image
</commit_message>
<xml_diff>
--- a/HolidayCoroOutlineCalculator.xlsx
+++ b/HolidayCoroOutlineCalculator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanbryant/Projects/house-lights/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A7BE91-C7B3-D945-B392-71D54580780F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0EA6DF-FBC0-6949-AE0F-08A7CBD77B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -343,9 +343,6 @@
     <t>Output Data for Each House Section</t>
   </si>
   <si>
-    <t>RGB Channels per Section</t>
-  </si>
-  <si>
     <t>DMX Channels per Section</t>
   </si>
   <si>
@@ -625,19 +622,22 @@
     <t>Left Angle, Right Side</t>
   </si>
   <si>
+    <t>Left Side of Garage</t>
+  </si>
+  <si>
+    <t>Top of Garage</t>
+  </si>
+  <si>
+    <t>Right Side of Garage</t>
+  </si>
+  <si>
+    <t>RGB Channels per Section (Pixels)</t>
+  </si>
+  <si>
     <t>Right Angle, Left Side</t>
   </si>
   <si>
-    <t>Right Angle, Right Side</t>
-  </si>
-  <si>
-    <t>Left Side of Garage</t>
-  </si>
-  <si>
-    <t>Top of Garage</t>
-  </si>
-  <si>
-    <t>Right Side of Garage</t>
+    <t>Rigth Angle, Right Side</t>
   </si>
 </sst>
 </file>
@@ -1781,7 +1781,7 @@
   <sheetData>
     <row r="5" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C5" s="75"/>
       <c r="D5" s="75"/>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="6" spans="2:14" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="77" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6" s="78"/>
       <c r="D6" s="78"/>
@@ -1837,24 +1837,24 @@
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I11" s="67" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I12" s="67"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" s="67" t="s">
         <v>91</v>
-      </c>
-      <c r="I13" s="67" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
@@ -1864,17 +1864,17 @@
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1897,7 +1897,7 @@
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F4" sqref="F4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1920,7 +1920,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="86" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="86"/>
       <c r="C1" s="86"/>
@@ -1956,7 +1956,7 @@
       <c r="H2" s="84"/>
       <c r="I2" s="85"/>
       <c r="J2" s="88" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K2" s="89"/>
       <c r="L2" s="89"/>
@@ -1964,11 +1964,11 @@
       <c r="N2" s="89"/>
       <c r="O2" s="90"/>
       <c r="P2" s="87" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q2" s="85"/>
     </row>
-    <row r="3" spans="1:19" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" s="2" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" s="14" t="s">
         <v>1</v>
@@ -1983,10 +1983,10 @@
         <v>3</v>
       </c>
       <c r="F3" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>41</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>42</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>11</v>
@@ -1995,464 +1995,488 @@
         <v>26</v>
       </c>
       <c r="J3" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="L3" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="M3" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="N3" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="O3" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>50</v>
       </c>
       <c r="P3" s="16"/>
       <c r="Q3" s="17"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="65" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" s="43">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C4" s="43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="21">
         <f>CONVERT(C4,"in","ft")+B4</f>
-        <v>1.0833333333333333</v>
+        <v>8</v>
       </c>
       <c r="E4" s="22">
         <f>CONVERT(D4,"ft","m")</f>
-        <v>0.33019999999999999</v>
+        <v>2.4384000000000001</v>
       </c>
       <c r="F4" s="21">
         <f>ROUNDUP((D4/CONVERT($B$28,"in","ft")),0)</f>
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="G4" s="21">
         <f>SUM(F4*3)</f>
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="H4" s="23">
         <f t="shared" ref="H4:H23" si="0">SUM(F4*$I$28)</f>
-        <v>2.88</v>
+        <v>17.28</v>
       </c>
       <c r="I4" s="24">
         <f t="shared" ref="I4:I23" si="1">SUM(F4*$H$28)</f>
-        <v>2.8311999999999999</v>
+        <v>16.987200000000001</v>
       </c>
       <c r="J4" s="25">
         <f>SUM(((H4/$E$28)*0.002525)*2)</f>
-        <v>1.212E-3</v>
+        <v>7.2720000000000007E-3</v>
       </c>
       <c r="K4" s="26">
         <f>SUM(((H4/$E$28)*0.00402)*2)</f>
-        <v>1.9296000000000001E-3</v>
+        <v>1.1577600000000002E-2</v>
       </c>
       <c r="L4" s="26">
         <f>SUM(((H4/$E$28)*0.00639)*2)</f>
-        <v>3.0672E-3</v>
+        <v>1.8403200000000002E-2</v>
       </c>
       <c r="M4" s="26">
         <f>SUM(((H4/$E$28)*0.01015)*2)</f>
-        <v>4.8719999999999996E-3</v>
+        <v>2.9232000000000001E-2</v>
       </c>
       <c r="N4" s="26">
         <f>SUM(((H4/$E$28)*0.01614)*2)</f>
-        <v>7.7472000000000001E-3</v>
+        <v>4.6483200000000009E-2</v>
       </c>
       <c r="O4" s="27">
         <f>SUM(((H4/$E$28)*0.02567)*2)</f>
-        <v>1.2321599999999999E-2</v>
+        <v>7.3929599999999998E-2</v>
       </c>
       <c r="P4" s="45" t="s">
         <v>33</v>
       </c>
       <c r="Q4" s="35">
         <f>SUM(F24)</f>
-        <v>4</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="65" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
+        <v>133</v>
+      </c>
+      <c r="B5" s="43">
+        <v>8</v>
+      </c>
+      <c r="C5" s="43">
+        <v>0</v>
+      </c>
       <c r="D5" s="21">
         <f t="shared" ref="D5:D11" si="2">CONVERT(C5,"in","ft")+B5</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E5" s="22">
         <f t="shared" ref="E5:E24" si="3">CONVERT(D5,"ft","m")</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
       <c r="F5" s="21">
         <f t="shared" ref="F5:F23" si="4">ROUNDUP((D5/CONVERT($B$28,"in","ft")),0)</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G5" s="21">
         <f t="shared" ref="G5:G23" si="5">SUM(F5*3)</f>
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="H5" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17.28</v>
       </c>
       <c r="I5" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>16.987200000000001</v>
       </c>
       <c r="J5" s="25">
         <f t="shared" ref="J5:J23" si="6">SUM(((H5/$E$28)*0.002525)*2)</f>
-        <v>0</v>
+        <v>7.2720000000000007E-3</v>
       </c>
       <c r="K5" s="26">
         <f t="shared" ref="K5:K23" si="7">SUM(((H5/$E$28)*0.00402)*2)</f>
-        <v>0</v>
+        <v>1.1577600000000002E-2</v>
       </c>
       <c r="L5" s="26">
         <f t="shared" ref="L5:L23" si="8">SUM(((H5/$E$28)*0.00639)*2)</f>
-        <v>0</v>
+        <v>1.8403200000000002E-2</v>
       </c>
       <c r="M5" s="26">
         <f t="shared" ref="M5:M23" si="9">SUM(((H5/$E$28)*0.01015)*2)</f>
-        <v>0</v>
+        <v>2.9232000000000001E-2</v>
       </c>
       <c r="N5" s="26">
         <f t="shared" ref="N5:N23" si="10">SUM(((H5/$E$28)*0.01614)*2)</f>
-        <v>0</v>
+        <v>4.6483200000000009E-2</v>
       </c>
       <c r="O5" s="27">
         <f t="shared" ref="O5:O23" si="11">SUM(((H5/$E$28)*0.02567)*2)</f>
-        <v>0</v>
+        <v>7.3929599999999998E-2</v>
       </c>
       <c r="P5" s="45" t="s">
         <v>34</v>
       </c>
       <c r="Q5" s="35">
         <f>ROUNDUP((F24/C28),0)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="65" t="s">
-        <v>135</v>
-      </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
+        <v>138</v>
+      </c>
+      <c r="B6" s="43">
+        <v>6</v>
+      </c>
+      <c r="C6" s="43">
+        <v>0</v>
+      </c>
       <c r="D6" s="21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E6" s="22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.8288</v>
       </c>
       <c r="F6" s="21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G6" s="21">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="H6" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12.959999999999999</v>
       </c>
       <c r="I6" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12.740399999999999</v>
       </c>
       <c r="J6" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5.4539999999999988E-3</v>
       </c>
       <c r="K6" s="26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>8.6831999999999986E-3</v>
       </c>
       <c r="L6" s="26">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.3802399999999998E-2</v>
       </c>
       <c r="M6" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>2.1923999999999996E-2</v>
       </c>
       <c r="N6" s="26">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3.4862400000000002E-2</v>
       </c>
       <c r="O6" s="27">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>5.5447199999999988E-2</v>
       </c>
       <c r="P6" s="45" t="s">
         <v>35</v>
       </c>
       <c r="Q6" s="35" t="str">
         <f>CONCATENATE(ROUND(H24,0)," Watts")</f>
-        <v>3 Watts</v>
+        <v>146 Watts</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="65" t="s">
-        <v>136</v>
-      </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
+        <v>139</v>
+      </c>
+      <c r="B7" s="43">
+        <v>13</v>
+      </c>
+      <c r="C7" s="43">
+        <v>7</v>
+      </c>
       <c r="D7" s="21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13.583333333333334</v>
       </c>
       <c r="E7" s="22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4.1402000000000001</v>
       </c>
       <c r="F7" s="21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="G7" s="21">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="H7" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>29.52</v>
       </c>
       <c r="I7" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>29.0198</v>
       </c>
       <c r="J7" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1.2423E-2</v>
       </c>
       <c r="K7" s="26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.9778400000000002E-2</v>
       </c>
       <c r="L7" s="26">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3.1438799999999996E-2</v>
       </c>
       <c r="M7" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4.9937999999999996E-2</v>
       </c>
       <c r="N7" s="26">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>7.9408800000000002E-2</v>
       </c>
       <c r="O7" s="27">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.1262964</v>
       </c>
       <c r="P7" s="45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q7" s="36" t="str">
         <f>CONCATENATE(ROUND(($H$24/5),0)," @ 5VDC")</f>
-        <v>1 @ 5VDC</v>
+        <v>29 @ 5VDC</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="65" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
+        <v>134</v>
+      </c>
+      <c r="B8" s="43">
+        <v>7</v>
+      </c>
+      <c r="C8" s="43">
+        <v>10</v>
+      </c>
       <c r="D8" s="21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.833333333333333</v>
       </c>
       <c r="E8" s="22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.3875999999999999</v>
       </c>
       <c r="F8" s="21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G8" s="21">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="H8" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17.28</v>
       </c>
       <c r="I8" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>16.987200000000001</v>
       </c>
       <c r="J8" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>7.2720000000000007E-3</v>
       </c>
       <c r="K8" s="26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.1577600000000002E-2</v>
       </c>
       <c r="L8" s="26">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.8403200000000002E-2</v>
       </c>
       <c r="M8" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>2.9232000000000001E-2</v>
       </c>
       <c r="N8" s="26">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>4.6483200000000009E-2</v>
       </c>
       <c r="O8" s="27">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>7.3929599999999998E-2</v>
       </c>
       <c r="P8" s="45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q8" s="36" t="str">
         <f>CONCATENATE(ROUND(($H$24/12),0)," @ 12VDC")</f>
-        <v>0 @ 12VDC</v>
+        <v>12 @ 12VDC</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="65" t="s">
-        <v>138</v>
-      </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
+        <v>135</v>
+      </c>
+      <c r="B9" s="43">
+        <v>16</v>
+      </c>
+      <c r="C9" s="43">
+        <v>0</v>
+      </c>
       <c r="D9" s="21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E9" s="22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4.8768000000000002</v>
       </c>
       <c r="F9" s="21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="G9" s="21">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="H9" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>34.56</v>
       </c>
       <c r="I9" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>33.974400000000003</v>
       </c>
       <c r="J9" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1.4544000000000001E-2</v>
       </c>
       <c r="K9" s="26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2.3155200000000004E-2</v>
       </c>
       <c r="L9" s="26">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3.6806400000000003E-2</v>
       </c>
       <c r="M9" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>5.8464000000000002E-2</v>
       </c>
       <c r="N9" s="26">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>9.2966400000000018E-2</v>
       </c>
       <c r="O9" s="27">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.1478592</v>
       </c>
       <c r="P9" s="45" t="s">
         <v>20</v>
       </c>
       <c r="Q9" s="35">
         <f>SUM(G24)</f>
-        <v>12</v>
+        <v>609</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="65" t="s">
-        <v>139</v>
-      </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
+        <v>136</v>
+      </c>
+      <c r="B10" s="43">
+        <v>7</v>
+      </c>
+      <c r="C10" s="43">
+        <v>10</v>
+      </c>
       <c r="D10" s="21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.833333333333333</v>
       </c>
       <c r="E10" s="22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.3875999999999999</v>
       </c>
       <c r="F10" s="21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G10" s="21">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="H10" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17.28</v>
       </c>
       <c r="I10" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>16.987200000000001</v>
       </c>
       <c r="J10" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>7.2720000000000007E-3</v>
       </c>
       <c r="K10" s="26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.1577600000000002E-2</v>
       </c>
       <c r="L10" s="26">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.8403200000000002E-2</v>
       </c>
       <c r="M10" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>2.9232000000000001E-2</v>
       </c>
       <c r="N10" s="26">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>4.6483200000000009E-2</v>
       </c>
       <c r="O10" s="27">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>7.3929599999999998E-2</v>
       </c>
       <c r="P10" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q10" s="37">
         <f>ROUNDUP((G24/510),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
@@ -3155,27 +3179,27 @@
       <c r="C24" s="48"/>
       <c r="D24" s="49">
         <f>SUM(D4:D23)</f>
-        <v>1.0833333333333333</v>
+        <v>67.25</v>
       </c>
       <c r="E24" s="50">
         <f t="shared" si="3"/>
-        <v>0.33019999999999999</v>
+        <v>20.497800000000002</v>
       </c>
       <c r="F24" s="49">
         <f>SUM(F4:F23)</f>
-        <v>4</v>
+        <v>203</v>
       </c>
       <c r="G24" s="49">
         <f>SUM(G4:G23)</f>
-        <v>12</v>
+        <v>609</v>
       </c>
       <c r="H24" s="51">
         <f>SUM(H4:H23)</f>
-        <v>2.88</v>
+        <v>146.16</v>
       </c>
       <c r="I24" s="52">
         <f>SUM(I4:I23)</f>
-        <v>2.8311999999999999</v>
+        <v>143.68340000000001</v>
       </c>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
@@ -3186,7 +3210,7 @@
     </row>
     <row r="26" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="83" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B26" s="83"/>
       <c r="C26" s="83"/>
@@ -3202,7 +3226,7 @@
     </row>
     <row r="27" spans="1:18" ht="64" x14ac:dyDescent="0.2">
       <c r="A27" s="40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>5</v>
@@ -3217,7 +3241,7 @@
         <v>9</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>13</v>
@@ -3243,7 +3267,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="61" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" s="38">
         <f>IF($A$28="","",INDEX('Pixel Data'!B$3:B$54,MATCH($A$28,'Pixel Data'!$A$3:$A$54,0)))</f>
@@ -3296,12 +3320,12 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -3412,7 +3436,7 @@
         <v>8</v>
       </c>
       <c r="M2" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
@@ -3420,7 +3444,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="72" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="20">
         <v>4</v>
@@ -3438,7 +3462,7 @@
         <v>60</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H3" s="55">
         <f t="shared" ref="H3:H32" si="0">SUM(D3/C3)</f>
@@ -3461,7 +3485,7 @@
         <v>50</v>
       </c>
       <c r="M3" s="64" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
@@ -3469,7 +3493,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="72" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="20">
         <v>2.44</v>
@@ -3487,7 +3511,7 @@
         <v>60</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H4" s="55">
         <f t="shared" si="0"/>
@@ -3510,7 +3534,7 @@
         <v>80</v>
       </c>
       <c r="M4" s="64" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
@@ -3518,7 +3542,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="72" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" s="20">
         <v>1.97</v>
@@ -3536,7 +3560,7 @@
         <v>60</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H5" s="55">
         <f t="shared" si="0"/>
@@ -3559,7 +3583,7 @@
         <v>100</v>
       </c>
       <c r="M5" s="64" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
@@ -3567,7 +3591,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="72" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="20">
         <v>4</v>
@@ -3585,7 +3609,7 @@
         <v>60</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H6" s="55">
         <f t="shared" si="0"/>
@@ -3608,7 +3632,7 @@
         <v>150</v>
       </c>
       <c r="M6" s="64" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
@@ -3616,7 +3640,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="72" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" s="20">
         <v>0.65</v>
@@ -3634,7 +3658,7 @@
         <v>60</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H7" s="55">
         <f t="shared" si="0"/>
@@ -3657,7 +3681,7 @@
         <v>300</v>
       </c>
       <c r="M7" s="64" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
@@ -3665,7 +3689,7 @@
     </row>
     <row r="8" spans="1:16" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="72" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B8" s="20">
         <v>8</v>
@@ -3683,7 +3707,7 @@
         <v>40</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H8" s="55">
         <f t="shared" si="0"/>
@@ -3706,7 +3730,7 @@
         <v>50</v>
       </c>
       <c r="M8" s="64" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
@@ -3714,7 +3738,7 @@
     </row>
     <row r="9" spans="1:16" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B9" s="20">
         <v>10</v>
@@ -3732,7 +3756,7 @@
         <v>40</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H9" s="55">
         <f t="shared" si="0"/>
@@ -3755,7 +3779,7 @@
         <v>50</v>
       </c>
       <c r="M9" s="64" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
@@ -3763,7 +3787,7 @@
     </row>
     <row r="10" spans="1:16" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="72" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B10" s="20">
         <v>12</v>
@@ -3781,7 +3805,7 @@
         <v>40</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H10" s="55">
         <f t="shared" si="0"/>
@@ -3804,7 +3828,7 @@
         <v>50</v>
       </c>
       <c r="M10" s="64" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
@@ -3812,7 +3836,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="71" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B11" s="20">
         <v>1</v>
@@ -3830,7 +3854,7 @@
         <v>60</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H11" s="55">
         <f t="shared" ref="H11:H22" si="5">SUM(D11/C11)</f>
@@ -3852,7 +3876,7 @@
         <v>1</v>
       </c>
       <c r="M11" s="64" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -3860,7 +3884,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="71" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B12" s="20">
         <v>2</v>
@@ -3878,7 +3902,7 @@
         <v>60</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H12" s="55">
         <f t="shared" si="5"/>
@@ -3900,7 +3924,7 @@
         <v>1</v>
       </c>
       <c r="M12" s="64" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
@@ -3908,7 +3932,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="71" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B13" s="20">
         <v>3</v>
@@ -3926,7 +3950,7 @@
         <v>60</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H13" s="55">
         <f t="shared" si="5"/>
@@ -3948,7 +3972,7 @@
         <v>1</v>
       </c>
       <c r="M13" s="64" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
@@ -3956,7 +3980,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="72" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14" s="20">
         <v>4</v>
@@ -3974,7 +3998,7 @@
         <v>60</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H14" s="55">
         <f t="shared" si="5"/>
@@ -3996,7 +4020,7 @@
         <v>1</v>
       </c>
       <c r="M14" s="64" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
@@ -4004,7 +4028,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="72" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B15" s="20">
         <v>5</v>
@@ -4022,7 +4046,7 @@
         <v>60</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H15" s="55">
         <f t="shared" si="5"/>
@@ -4044,7 +4068,7 @@
         <v>1</v>
       </c>
       <c r="M15" s="64" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
@@ -4052,7 +4076,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="72" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B16" s="20">
         <v>6</v>
@@ -4070,7 +4094,7 @@
         <v>60</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H16" s="55">
         <f t="shared" si="5"/>
@@ -4092,7 +4116,7 @@
         <v>1</v>
       </c>
       <c r="M16" s="64" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
@@ -4100,7 +4124,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="71" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B17" s="20">
         <v>1</v>
@@ -4118,7 +4142,7 @@
         <v>60</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H17" s="55">
         <f t="shared" si="5"/>
@@ -4140,7 +4164,7 @@
         <v>1</v>
       </c>
       <c r="M17" s="64" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
@@ -4148,7 +4172,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="71" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B18" s="20">
         <v>2</v>
@@ -4166,7 +4190,7 @@
         <v>60</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H18" s="55">
         <f t="shared" si="5"/>
@@ -4188,7 +4212,7 @@
         <v>1</v>
       </c>
       <c r="M18" s="64" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
@@ -4196,7 +4220,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="71" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B19" s="20">
         <v>3</v>
@@ -4214,7 +4238,7 @@
         <v>60</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H19" s="55">
         <f t="shared" si="5"/>
@@ -4236,7 +4260,7 @@
         <v>1</v>
       </c>
       <c r="M19" s="64" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
@@ -4244,7 +4268,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="72" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B20" s="20">
         <v>1</v>
@@ -4262,7 +4286,7 @@
         <v>60</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H20" s="55">
         <f t="shared" si="5"/>
@@ -4285,7 +4309,7 @@
         <v>1</v>
       </c>
       <c r="M20" s="64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
@@ -4293,7 +4317,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="72" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B21" s="20">
         <v>2</v>
@@ -4311,7 +4335,7 @@
         <v>60</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H21" s="55">
         <f t="shared" si="5"/>
@@ -4334,7 +4358,7 @@
         <v>1</v>
       </c>
       <c r="M21" s="64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
@@ -4342,7 +4366,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="72" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B22" s="20">
         <v>3</v>
@@ -4360,7 +4384,7 @@
         <v>60</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H22" s="55">
         <f t="shared" si="5"/>
@@ -4383,7 +4407,7 @@
         <v>1</v>
       </c>
       <c r="M22" s="64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
@@ -4391,7 +4415,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="71" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B23" s="20">
         <v>1</v>
@@ -4409,7 +4433,7 @@
         <v>60</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H23" s="55">
         <f t="shared" ref="H23" si="10">SUM(D23/C23)</f>
@@ -4432,7 +4456,7 @@
         <v>1</v>
       </c>
       <c r="M23" s="64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
@@ -4440,7 +4464,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="71" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B24" s="20">
         <v>2</v>
@@ -4458,7 +4482,7 @@
         <v>60</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H24" s="55">
         <f t="shared" ref="H24:H25" si="15">SUM(D24/C24)</f>
@@ -4481,7 +4505,7 @@
         <v>1</v>
       </c>
       <c r="M24" s="64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
@@ -4489,7 +4513,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="71" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B25" s="20">
         <v>3</v>
@@ -4507,7 +4531,7 @@
         <v>60</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H25" s="55">
         <f t="shared" si="15"/>
@@ -4530,7 +4554,7 @@
         <v>1</v>
       </c>
       <c r="M25" s="64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
@@ -4538,7 +4562,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="71" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B26" s="20">
         <v>3</v>
@@ -4556,7 +4580,7 @@
         <v>64</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H26" s="55">
         <f>SUM(D26/C26)</f>
@@ -4579,7 +4603,7 @@
         <v>1</v>
       </c>
       <c r="M26" s="64" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
@@ -4587,7 +4611,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="71" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B27" s="20">
         <v>3</v>
@@ -4605,7 +4629,7 @@
         <v>64</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H27" s="55">
         <f>SUM(D27/C27)</f>
@@ -4628,7 +4652,7 @@
         <v>1</v>
       </c>
       <c r="M27" s="64" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
@@ -4636,7 +4660,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="43"/>
       <c r="C28" s="43"/>
@@ -4671,7 +4695,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B29" s="43"/>
       <c r="C29" s="43"/>
@@ -4706,7 +4730,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="43"/>
       <c r="C30" s="43"/>
@@ -4741,7 +4765,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31" s="43"/>
       <c r="C31" s="43"/>
@@ -4776,7 +4800,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B32" s="43"/>
       <c r="C32" s="43"/>
@@ -4811,7 +4835,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33" s="43"/>
       <c r="C33" s="43"/>
@@ -4846,7 +4870,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" s="43"/>
       <c r="C34" s="43"/>
@@ -4881,7 +4905,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" s="43"/>
       <c r="C35" s="43"/>
@@ -4916,7 +4940,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" s="43"/>
       <c r="C36" s="43"/>
@@ -4951,7 +4975,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" s="43"/>
       <c r="C37" s="43"/>
@@ -4986,7 +5010,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38" s="43"/>
       <c r="C38" s="43"/>
@@ -5021,7 +5045,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="43"/>
       <c r="C39" s="43"/>
@@ -5056,7 +5080,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B40" s="43"/>
       <c r="C40" s="43"/>
@@ -5091,7 +5115,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B41" s="43"/>
       <c r="C41" s="43"/>
@@ -5126,7 +5150,7 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B42" s="43"/>
       <c r="C42" s="43"/>
@@ -5161,7 +5185,7 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43" s="43"/>
       <c r="C43" s="43"/>
@@ -5196,7 +5220,7 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B44" s="43"/>
       <c r="C44" s="43"/>
@@ -5231,7 +5255,7 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45" s="43"/>
       <c r="C45" s="43"/>
@@ -5266,7 +5290,7 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B46" s="43"/>
       <c r="C46" s="43"/>
@@ -5301,7 +5325,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B47" s="43"/>
       <c r="C47" s="43"/>
@@ -5336,7 +5360,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48" s="43"/>
       <c r="C48" s="43"/>
@@ -5371,7 +5395,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B49" s="43"/>
       <c r="C49" s="43"/>
@@ -5406,7 +5430,7 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50" s="43"/>
       <c r="C50" s="43"/>
@@ -5441,7 +5465,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" s="43"/>
       <c r="C51" s="43"/>
@@ -5476,7 +5500,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" s="43"/>
       <c r="C52" s="43"/>
@@ -5511,7 +5535,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" s="43"/>
       <c r="C53" s="43"/>
@@ -5546,7 +5570,7 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54" s="43"/>
       <c r="C54" s="43"/>
@@ -5611,7 +5635,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5621,7 +5645,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="92" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="92"/>
       <c r="C1" s="92"/>
@@ -5658,7 +5682,7 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -5666,7 +5690,7 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -5679,10 +5703,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
         <v>73</v>
-      </c>
-      <c r="B7" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -5690,31 +5714,31 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
         <v>59</v>
-      </c>
-      <c r="B9" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
         <v>62</v>
-      </c>
-      <c r="B10" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" t="s">
         <v>64</v>
-      </c>
-      <c r="B11" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update image and finalize Excel calculator.
</commit_message>
<xml_diff>
--- a/HolidayCoroOutlineCalculator.xlsx
+++ b/HolidayCoroOutlineCalculator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanbryant/Projects/house-lights/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryant/Development/house-lights/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0EA6DF-FBC0-6949-AE0F-08A7CBD77B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB713EAF-750A-F347-A8A9-9933CC0D10BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="5" r:id="rId1"/>
@@ -55,7 +55,7 @@
           <rPr>
             <b/>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -648,7 +648,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -730,6 +730,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1133,7 +1140,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1147,19 +1154,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1178,10 +1185,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1263,12 +1270,6 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1327,12 +1328,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1353,17 +1348,13 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1376,7 +1367,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1780,55 +1771,55 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="68" t="s">
         <v>122</v>
       </c>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="75"/>
-      <c r="N5" s="76"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="70"/>
     </row>
     <row r="6" spans="2:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="B6" s="77" t="s">
+      <c r="B6" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="79"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
+      <c r="N6" s="73"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B7" s="80">
+      <c r="B7" s="74">
         <v>42241</v>
       </c>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="81"/>
-      <c r="I7" s="81"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="82"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="76"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
@@ -1839,7 +1830,7 @@
       <c r="B11" t="s">
         <v>119</v>
       </c>
-      <c r="I11" s="67" t="s">
+      <c r="I11" s="63" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1847,13 +1838,13 @@
       <c r="B12" t="s">
         <v>120</v>
       </c>
-      <c r="I12" s="67"/>
+      <c r="I12" s="63"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>90</v>
       </c>
-      <c r="I13" s="67" t="s">
+      <c r="I13" s="63" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1897,7 +1888,7 @@
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1919,54 +1910,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="80" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="86"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="80"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84" t="s">
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="88" t="s">
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="87" t="s">
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="Q2" s="85"/>
+      <c r="Q2" s="79"/>
     </row>
     <row r="3" spans="1:19" s="2" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
@@ -2016,13 +2007,13 @@
       <c r="Q3" s="17"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="61" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="43">
+      <c r="B4" s="41">
         <v>8</v>
       </c>
-      <c r="C4" s="43">
+      <c r="C4" s="41">
         <v>0</v>
       </c>
       <c r="D4" s="21">
@@ -2073,22 +2064,22 @@
         <f>SUM(((H4/$E$28)*0.02567)*2)</f>
         <v>7.3929599999999998E-2</v>
       </c>
-      <c r="P4" s="45" t="s">
+      <c r="P4" s="43" t="s">
         <v>33</v>
       </c>
       <c r="Q4" s="35">
         <f>SUM(F24)</f>
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="B5" s="43">
+      <c r="B5" s="41">
         <v>8</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="41">
         <v>0</v>
       </c>
       <c r="D5" s="21">
@@ -2139,7 +2130,7 @@
         <f t="shared" ref="O5:O23" si="11">SUM(((H5/$E$28)*0.02567)*2)</f>
         <v>7.3929599999999998E-2</v>
       </c>
-      <c r="P5" s="45" t="s">
+      <c r="P5" s="43" t="s">
         <v>34</v>
       </c>
       <c r="Q5" s="35">
@@ -2150,145 +2141,145 @@
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="61" t="s">
         <v>138</v>
       </c>
-      <c r="B6" s="43">
+      <c r="B6" s="41">
         <v>6</v>
       </c>
-      <c r="C6" s="43">
-        <v>0</v>
+      <c r="C6" s="41">
+        <v>4</v>
       </c>
       <c r="D6" s="21">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>6.333333333333333</v>
       </c>
       <c r="E6" s="22">
         <f t="shared" si="3"/>
-        <v>1.8288</v>
+        <v>1.9303999999999999</v>
       </c>
       <c r="F6" s="21">
         <f t="shared" si="4"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G6" s="21">
         <f t="shared" si="5"/>
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H6" s="23">
         <f t="shared" si="0"/>
-        <v>12.959999999999999</v>
+        <v>13.68</v>
       </c>
       <c r="I6" s="24">
         <f t="shared" si="1"/>
-        <v>12.740399999999999</v>
+        <v>13.4482</v>
       </c>
       <c r="J6" s="25">
         <f t="shared" si="6"/>
-        <v>5.4539999999999988E-3</v>
+        <v>5.7569999999999991E-3</v>
       </c>
       <c r="K6" s="26">
         <f t="shared" si="7"/>
-        <v>8.6831999999999986E-3</v>
+        <v>9.1655999999999994E-3</v>
       </c>
       <c r="L6" s="26">
         <f t="shared" si="8"/>
-        <v>1.3802399999999998E-2</v>
+        <v>1.4569199999999999E-2</v>
       </c>
       <c r="M6" s="26">
         <f t="shared" si="9"/>
-        <v>2.1923999999999996E-2</v>
+        <v>2.3141999999999996E-2</v>
       </c>
       <c r="N6" s="26">
         <f t="shared" si="10"/>
-        <v>3.4862400000000002E-2</v>
+        <v>3.6799199999999997E-2</v>
       </c>
       <c r="O6" s="27">
         <f t="shared" si="11"/>
-        <v>5.5447199999999988E-2</v>
-      </c>
-      <c r="P6" s="45" t="s">
+        <v>5.8527599999999992E-2</v>
+      </c>
+      <c r="P6" s="43" t="s">
         <v>35</v>
       </c>
       <c r="Q6" s="35" t="str">
         <f>CONCATENATE(ROUND(H24,0)," Watts")</f>
-        <v>146 Watts</v>
+        <v>148 Watts</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="61" t="s">
         <v>139</v>
       </c>
-      <c r="B7" s="43">
-        <v>13</v>
-      </c>
-      <c r="C7" s="43">
-        <v>7</v>
+      <c r="B7" s="41">
+        <v>14</v>
+      </c>
+      <c r="C7" s="41">
+        <v>4</v>
       </c>
       <c r="D7" s="21">
         <f t="shared" si="2"/>
-        <v>13.583333333333334</v>
+        <v>14.333333333333334</v>
       </c>
       <c r="E7" s="22">
         <f t="shared" si="3"/>
-        <v>4.1402000000000001</v>
+        <v>4.3688000000000002</v>
       </c>
       <c r="F7" s="21">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G7" s="21">
         <f t="shared" si="5"/>
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="H7" s="23">
         <f t="shared" si="0"/>
-        <v>29.52</v>
+        <v>30.959999999999997</v>
       </c>
       <c r="I7" s="24">
         <f t="shared" si="1"/>
-        <v>29.0198</v>
+        <v>30.435399999999998</v>
       </c>
       <c r="J7" s="25">
         <f t="shared" si="6"/>
-        <v>1.2423E-2</v>
+        <v>1.3028999999999997E-2</v>
       </c>
       <c r="K7" s="26">
         <f t="shared" si="7"/>
-        <v>1.9778400000000002E-2</v>
+        <v>2.0743199999999996E-2</v>
       </c>
       <c r="L7" s="26">
         <f t="shared" si="8"/>
-        <v>3.1438799999999996E-2</v>
+        <v>3.2972399999999992E-2</v>
       </c>
       <c r="M7" s="26">
         <f t="shared" si="9"/>
-        <v>4.9937999999999996E-2</v>
+        <v>5.237399999999999E-2</v>
       </c>
       <c r="N7" s="26">
         <f t="shared" si="10"/>
-        <v>7.9408800000000002E-2</v>
+        <v>8.3282399999999993E-2</v>
       </c>
       <c r="O7" s="27">
         <f t="shared" si="11"/>
-        <v>0.1262964</v>
-      </c>
-      <c r="P7" s="45" t="s">
+        <v>0.13245719999999997</v>
+      </c>
+      <c r="P7" s="43" t="s">
         <v>42</v>
       </c>
       <c r="Q7" s="36" t="str">
         <f>CONCATENATE(ROUND(($H$24/5),0)," @ 5VDC")</f>
-        <v>29 @ 5VDC</v>
+        <v>30 @ 5VDC</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="B8" s="43">
+      <c r="B8" s="41">
         <v>7</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="41">
         <v>10</v>
       </c>
       <c r="D8" s="21">
@@ -2339,7 +2330,7 @@
         <f t="shared" si="11"/>
         <v>7.3929599999999998E-2</v>
       </c>
-      <c r="P8" s="45" t="s">
+      <c r="P8" s="43" t="s">
         <v>43</v>
       </c>
       <c r="Q8" s="36" t="str">
@@ -2348,13 +2339,13 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="61" t="s">
         <v>135</v>
       </c>
-      <c r="B9" s="43">
+      <c r="B9" s="41">
         <v>16</v>
       </c>
-      <c r="C9" s="43">
+      <c r="C9" s="41">
         <v>0</v>
       </c>
       <c r="D9" s="21">
@@ -2405,22 +2396,22 @@
         <f t="shared" si="11"/>
         <v>0.1478592</v>
       </c>
-      <c r="P9" s="45" t="s">
+      <c r="P9" s="43" t="s">
         <v>20</v>
       </c>
       <c r="Q9" s="35">
         <f>SUM(G24)</f>
-        <v>609</v>
+        <v>618</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="B10" s="43">
+      <c r="B10" s="41">
         <v>7</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="41">
         <v>10</v>
       </c>
       <c r="D10" s="21">
@@ -2471,7 +2462,7 @@
         <f t="shared" si="11"/>
         <v>7.3929599999999998E-2</v>
       </c>
-      <c r="P10" s="46" t="s">
+      <c r="P10" s="44" t="s">
         <v>70</v>
       </c>
       <c r="Q10" s="37">
@@ -2480,9 +2471,9 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="65"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
+      <c r="A11" s="61"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="21">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2533,9 +2524,9 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="65"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="21">
         <f>CONVERT(C12,"in","ft")+B12</f>
         <v>0</v>
@@ -2586,9 +2577,9 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="65"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
       <c r="D13" s="21">
         <f>CONVERT(C13,"in","ft")+B13</f>
         <v>0</v>
@@ -2639,9 +2630,9 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="65"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
+      <c r="A14" s="61"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
       <c r="D14" s="21">
         <f t="shared" ref="D14:D23" si="12">CONVERT(C14,"in","ft")+B14</f>
         <v>0</v>
@@ -2692,9 +2683,9 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="65"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
+      <c r="A15" s="61"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
       <c r="D15" s="21">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -2745,9 +2736,9 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="65"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
       <c r="D16" s="21">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -2798,9 +2789,9 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="65"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
+      <c r="A17" s="61"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
       <c r="D17" s="21">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -2851,9 +2842,9 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="65"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
+      <c r="A18" s="61"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
       <c r="D18" s="21">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -2905,9 +2896,9 @@
       <c r="Q18" s="8"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A19" s="65"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
+      <c r="A19" s="61"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
       <c r="D19" s="21">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -2958,9 +2949,9 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A20" s="65"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
       <c r="D20" s="21">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -3013,9 +3004,9 @@
       <c r="R20" s="3"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" s="65"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
+      <c r="A21" s="61"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
       <c r="D21" s="21">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -3066,9 +3057,9 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" s="65"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
+      <c r="A22" s="61"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
       <c r="D22" s="21">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -3119,9 +3110,9 @@
       </c>
     </row>
     <row r="23" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="66"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
+      <c r="A23" s="62"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
       <c r="D23" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -3172,34 +3163,34 @@
       </c>
     </row>
     <row r="24" spans="1:18" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="47" t="s">
+      <c r="A24" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="48"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="49">
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="47">
         <f>SUM(D4:D23)</f>
-        <v>67.25</v>
-      </c>
-      <c r="E24" s="50">
+        <v>68.333333333333329</v>
+      </c>
+      <c r="E24" s="48">
         <f t="shared" si="3"/>
-        <v>20.497800000000002</v>
-      </c>
-      <c r="F24" s="49">
+        <v>20.827999999999999</v>
+      </c>
+      <c r="F24" s="47">
         <f>SUM(F4:F23)</f>
-        <v>203</v>
-      </c>
-      <c r="G24" s="49">
+        <v>206</v>
+      </c>
+      <c r="G24" s="47">
         <f>SUM(G4:G23)</f>
-        <v>609</v>
-      </c>
-      <c r="H24" s="51">
+        <v>618</v>
+      </c>
+      <c r="H24" s="49">
         <f>SUM(H4:H23)</f>
-        <v>146.16</v>
-      </c>
-      <c r="I24" s="52">
+        <v>148.32000000000002</v>
+      </c>
+      <c r="I24" s="50">
         <f>SUM(I4:I23)</f>
-        <v>143.68340000000001</v>
+        <v>145.80680000000001</v>
       </c>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
@@ -3209,23 +3200,23 @@
       <c r="O24" s="18"/>
     </row>
     <row r="26" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="83" t="s">
+      <c r="A26" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="83"/>
-      <c r="C26" s="83"/>
-      <c r="D26" s="83"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="83"/>
-      <c r="G26" s="83"/>
-      <c r="H26" s="83"/>
-      <c r="I26" s="83"/>
-      <c r="J26" s="83"/>
-      <c r="K26" s="83"/>
-      <c r="L26" s="83"/>
+      <c r="B26" s="77"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="77"/>
+      <c r="H26" s="77"/>
+      <c r="I26" s="77"/>
+      <c r="J26" s="77"/>
+      <c r="K26" s="77"/>
+      <c r="L26" s="77"/>
     </row>
     <row r="27" spans="1:18" ht="64" x14ac:dyDescent="0.2">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="7" t="s">
         <v>67</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -3266,7 +3257,7 @@
       <c r="O27" s="7"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A28" s="61" t="s">
+      <c r="A28" s="57" t="s">
         <v>97</v>
       </c>
       <c r="B28" s="38">
@@ -3313,10 +3304,10 @@
         <f>IF($A$28="","",INDEX('Pixel Data'!L$3:L$54,MATCH($A$28,'Pixel Data'!$A$3:$A$54,0)))</f>
         <v>50</v>
       </c>
-      <c r="N28" s="69"/>
+      <c r="N28" s="64"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N29" s="70"/>
+      <c r="N29" s="65"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -3370,72 +3361,72 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="83.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="68" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="68" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" style="68" customWidth="1"/>
-    <col min="7" max="7" width="14.5" style="68" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="41" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.5" style="68" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.1640625" style="68"/>
+    <col min="5" max="6" width="10.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.1640625" style="1"/>
     <col min="13" max="13" width="45.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="58" t="s">
+      <c r="H2" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="57" t="s">
+      <c r="I2" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="57" t="s">
+      <c r="K2" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="57" t="s">
+      <c r="L2" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="56" t="s">
+      <c r="M2" s="54" t="s">
         <v>53</v>
       </c>
       <c r="N2" s="4"/>
@@ -3443,7 +3434,7 @@
       <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="67" t="s">
         <v>97</v>
       </c>
       <c r="B3" s="20">
@@ -3452,19 +3443,19 @@
       <c r="C3" s="20">
         <v>50</v>
       </c>
-      <c r="D3" s="62">
+      <c r="D3" s="58">
         <v>35.39</v>
       </c>
       <c r="E3" s="20">
         <v>12</v>
       </c>
-      <c r="F3" s="63">
+      <c r="F3" s="59">
         <v>60</v>
       </c>
       <c r="G3" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="55">
+      <c r="H3" s="53">
         <f t="shared" ref="H3:H32" si="0">SUM(D3/C3)</f>
         <v>0.70779999999999998</v>
       </c>
@@ -3484,7 +3475,7 @@
         <f t="shared" ref="L3:L54" si="3">SUM(C3)</f>
         <v>50</v>
       </c>
-      <c r="M3" s="64" t="s">
+      <c r="M3" s="60" t="s">
         <v>74</v>
       </c>
       <c r="N3" s="5"/>
@@ -3492,7 +3483,7 @@
       <c r="P3" s="5"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="67" t="s">
         <v>98</v>
       </c>
       <c r="B4" s="20">
@@ -3501,19 +3492,19 @@
       <c r="C4" s="20">
         <v>80</v>
       </c>
-      <c r="D4" s="62">
+      <c r="D4" s="58">
         <v>46.99</v>
       </c>
       <c r="E4" s="20">
         <v>12</v>
       </c>
-      <c r="F4" s="63">
+      <c r="F4" s="59">
         <v>60</v>
       </c>
       <c r="G4" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="H4" s="55">
+      <c r="H4" s="53">
         <f t="shared" si="0"/>
         <v>0.58737499999999998</v>
       </c>
@@ -3533,7 +3524,7 @@
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="M4" s="64" t="s">
+      <c r="M4" s="60" t="s">
         <v>75</v>
       </c>
       <c r="N4" s="5"/>
@@ -3541,7 +3532,7 @@
       <c r="P4" s="5"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="67" t="s">
         <v>99</v>
       </c>
       <c r="B5" s="20">
@@ -3550,19 +3541,19 @@
       <c r="C5" s="20">
         <v>100</v>
       </c>
-      <c r="D5" s="62">
+      <c r="D5" s="58">
         <v>48.37</v>
       </c>
       <c r="E5" s="20">
         <v>12</v>
       </c>
-      <c r="F5" s="63">
+      <c r="F5" s="59">
         <v>60</v>
       </c>
       <c r="G5" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="H5" s="55">
+      <c r="H5" s="53">
         <f t="shared" si="0"/>
         <v>0.48369999999999996</v>
       </c>
@@ -3582,7 +3573,7 @@
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="M5" s="64" t="s">
+      <c r="M5" s="60" t="s">
         <v>76</v>
       </c>
       <c r="N5" s="5"/>
@@ -3590,7 +3581,7 @@
       <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="67" t="s">
         <v>100</v>
       </c>
       <c r="B6" s="20">
@@ -3599,19 +3590,19 @@
       <c r="C6" s="20">
         <v>150</v>
       </c>
-      <c r="D6" s="62">
+      <c r="D6" s="58">
         <v>47.49</v>
       </c>
       <c r="E6" s="20">
         <v>12</v>
       </c>
-      <c r="F6" s="63">
+      <c r="F6" s="59">
         <v>60</v>
       </c>
       <c r="G6" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="H6" s="55">
+      <c r="H6" s="53">
         <f t="shared" si="0"/>
         <v>0.31659999999999999</v>
       </c>
@@ -3631,7 +3622,7 @@
         <f t="shared" si="3"/>
         <v>150</v>
       </c>
-      <c r="M6" s="64" t="s">
+      <c r="M6" s="60" t="s">
         <v>93</v>
       </c>
       <c r="N6" s="5"/>
@@ -3639,7 +3630,7 @@
       <c r="P6" s="5"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="67" t="s">
         <v>101</v>
       </c>
       <c r="B7" s="20">
@@ -3648,19 +3639,19 @@
       <c r="C7" s="20">
         <v>300</v>
       </c>
-      <c r="D7" s="62">
+      <c r="D7" s="58">
         <v>64.989999999999995</v>
       </c>
       <c r="E7" s="20">
         <v>12</v>
       </c>
-      <c r="F7" s="63">
+      <c r="F7" s="59">
         <v>60</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="55">
+      <c r="H7" s="53">
         <f t="shared" si="0"/>
         <v>0.21663333333333332</v>
       </c>
@@ -3680,15 +3671,15 @@
         <f t="shared" si="3"/>
         <v>300</v>
       </c>
-      <c r="M7" s="64" t="s">
+      <c r="M7" s="60" t="s">
         <v>94</v>
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:16" s="73" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="72" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="67" t="s">
         <v>129</v>
       </c>
       <c r="B8" s="20">
@@ -3697,19 +3688,19 @@
       <c r="C8" s="20">
         <v>50</v>
       </c>
-      <c r="D8" s="62">
+      <c r="D8" s="58">
         <v>42.99</v>
       </c>
       <c r="E8" s="20">
         <v>12</v>
       </c>
-      <c r="F8" s="63">
+      <c r="F8" s="59">
         <v>40</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="H8" s="55">
+      <c r="H8" s="53">
         <f t="shared" si="0"/>
         <v>0.85980000000000001</v>
       </c>
@@ -3729,15 +3720,15 @@
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="M8" s="64" t="s">
+      <c r="M8" s="60" t="s">
         <v>128</v>
       </c>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:16" s="73" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="72" t="s">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="67" t="s">
         <v>130</v>
       </c>
       <c r="B9" s="20">
@@ -3746,19 +3737,19 @@
       <c r="C9" s="20">
         <v>50</v>
       </c>
-      <c r="D9" s="62">
+      <c r="D9" s="58">
         <v>43.99</v>
       </c>
       <c r="E9" s="20">
         <v>12</v>
       </c>
-      <c r="F9" s="63">
+      <c r="F9" s="59">
         <v>40</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="H9" s="55">
+      <c r="H9" s="53">
         <f t="shared" si="0"/>
         <v>0.87980000000000003</v>
       </c>
@@ -3778,15 +3769,15 @@
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="M9" s="64" t="s">
+      <c r="M9" s="60" t="s">
         <v>128</v>
       </c>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="1:16" s="73" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="72" t="s">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="67" t="s">
         <v>131</v>
       </c>
       <c r="B10" s="20">
@@ -3795,19 +3786,19 @@
       <c r="C10" s="20">
         <v>50</v>
       </c>
-      <c r="D10" s="62">
+      <c r="D10" s="58">
         <v>44.99</v>
       </c>
       <c r="E10" s="20">
         <v>12</v>
       </c>
-      <c r="F10" s="63">
+      <c r="F10" s="59">
         <v>40</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="H10" s="55">
+      <c r="H10" s="53">
         <f t="shared" si="0"/>
         <v>0.89980000000000004</v>
       </c>
@@ -3827,7 +3818,7 @@
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="M10" s="64" t="s">
+      <c r="M10" s="60" t="s">
         <v>128</v>
       </c>
       <c r="N10" s="5"/>
@@ -3835,7 +3826,7 @@
       <c r="P10" s="5"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="71" t="s">
+      <c r="A11" s="66" t="s">
         <v>102</v>
       </c>
       <c r="B11" s="20">
@@ -3844,19 +3835,19 @@
       <c r="C11" s="20">
         <v>1</v>
       </c>
-      <c r="D11" s="62">
+      <c r="D11" s="58">
         <v>0.47</v>
       </c>
       <c r="E11" s="20">
         <v>12</v>
       </c>
-      <c r="F11" s="63">
+      <c r="F11" s="59">
         <v>60</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H11" s="55">
+      <c r="H11" s="53">
         <f t="shared" ref="H11:H22" si="5">SUM(D11/C11)</f>
         <v>0.47</v>
       </c>
@@ -3875,7 +3866,7 @@
         <f t="shared" ref="L11:L22" si="8">SUM(C11)</f>
         <v>1</v>
       </c>
-      <c r="M11" s="64" t="s">
+      <c r="M11" s="60" t="s">
         <v>82</v>
       </c>
       <c r="N11" s="5"/>
@@ -3883,7 +3874,7 @@
       <c r="P11" s="5"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="71" t="s">
+      <c r="A12" s="66" t="s">
         <v>103</v>
       </c>
       <c r="B12" s="20">
@@ -3892,19 +3883,19 @@
       <c r="C12" s="20">
         <v>1</v>
       </c>
-      <c r="D12" s="62">
+      <c r="D12" s="58">
         <v>0.47</v>
       </c>
       <c r="E12" s="20">
         <v>12</v>
       </c>
-      <c r="F12" s="63">
+      <c r="F12" s="59">
         <v>60</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H12" s="55">
+      <c r="H12" s="53">
         <f t="shared" si="5"/>
         <v>0.47</v>
       </c>
@@ -3923,7 +3914,7 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="M12" s="64" t="s">
+      <c r="M12" s="60" t="s">
         <v>82</v>
       </c>
       <c r="N12" s="5"/>
@@ -3931,7 +3922,7 @@
       <c r="P12" s="5"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="71" t="s">
+      <c r="A13" s="66" t="s">
         <v>104</v>
       </c>
       <c r="B13" s="20">
@@ -3940,19 +3931,19 @@
       <c r="C13" s="20">
         <v>1</v>
       </c>
-      <c r="D13" s="62">
+      <c r="D13" s="58">
         <v>0.47</v>
       </c>
       <c r="E13" s="20">
         <v>12</v>
       </c>
-      <c r="F13" s="63">
+      <c r="F13" s="59">
         <v>60</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H13" s="55">
+      <c r="H13" s="53">
         <f t="shared" si="5"/>
         <v>0.47</v>
       </c>
@@ -3971,7 +3962,7 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="M13" s="64" t="s">
+      <c r="M13" s="60" t="s">
         <v>82</v>
       </c>
       <c r="N13" s="5"/>
@@ -3979,7 +3970,7 @@
       <c r="P13" s="5"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="72" t="s">
+      <c r="A14" s="67" t="s">
         <v>105</v>
       </c>
       <c r="B14" s="20">
@@ -3988,19 +3979,19 @@
       <c r="C14" s="20">
         <v>1</v>
       </c>
-      <c r="D14" s="62">
+      <c r="D14" s="58">
         <v>0.49</v>
       </c>
       <c r="E14" s="20">
         <v>12</v>
       </c>
-      <c r="F14" s="63">
+      <c r="F14" s="59">
         <v>60</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H14" s="55">
+      <c r="H14" s="53">
         <f t="shared" si="5"/>
         <v>0.49</v>
       </c>
@@ -4019,7 +4010,7 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="M14" s="64" t="s">
+      <c r="M14" s="60" t="s">
         <v>92</v>
       </c>
       <c r="N14" s="5"/>
@@ -4027,7 +4018,7 @@
       <c r="P14" s="5"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="72" t="s">
+      <c r="A15" s="67" t="s">
         <v>106</v>
       </c>
       <c r="B15" s="20">
@@ -4036,19 +4027,19 @@
       <c r="C15" s="20">
         <v>1</v>
       </c>
-      <c r="D15" s="62">
+      <c r="D15" s="58">
         <v>0.49</v>
       </c>
       <c r="E15" s="20">
         <v>12</v>
       </c>
-      <c r="F15" s="63">
+      <c r="F15" s="59">
         <v>60</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H15" s="55">
+      <c r="H15" s="53">
         <f t="shared" si="5"/>
         <v>0.49</v>
       </c>
@@ -4067,7 +4058,7 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="M15" s="64" t="s">
+      <c r="M15" s="60" t="s">
         <v>92</v>
       </c>
       <c r="N15" s="5"/>
@@ -4075,7 +4066,7 @@
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="72" t="s">
+      <c r="A16" s="67" t="s">
         <v>107</v>
       </c>
       <c r="B16" s="20">
@@ -4084,19 +4075,19 @@
       <c r="C16" s="20">
         <v>1</v>
       </c>
-      <c r="D16" s="62">
+      <c r="D16" s="58">
         <v>0.49</v>
       </c>
       <c r="E16" s="20">
         <v>12</v>
       </c>
-      <c r="F16" s="63">
+      <c r="F16" s="59">
         <v>60</v>
       </c>
       <c r="G16" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H16" s="55">
+      <c r="H16" s="53">
         <f t="shared" si="5"/>
         <v>0.49</v>
       </c>
@@ -4115,7 +4106,7 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="M16" s="64" t="s">
+      <c r="M16" s="60" t="s">
         <v>92</v>
       </c>
       <c r="N16" s="5"/>
@@ -4123,7 +4114,7 @@
       <c r="P16" s="5"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="71" t="s">
+      <c r="A17" s="66" t="s">
         <v>108</v>
       </c>
       <c r="B17" s="20">
@@ -4132,19 +4123,19 @@
       <c r="C17" s="20">
         <v>1</v>
       </c>
-      <c r="D17" s="62">
+      <c r="D17" s="58">
         <v>0.47</v>
       </c>
       <c r="E17" s="20">
         <v>12</v>
       </c>
-      <c r="F17" s="63">
+      <c r="F17" s="59">
         <v>60</v>
       </c>
       <c r="G17" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H17" s="55">
+      <c r="H17" s="53">
         <f t="shared" si="5"/>
         <v>0.47</v>
       </c>
@@ -4163,7 +4154,7 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="M17" s="64" t="s">
+      <c r="M17" s="60" t="s">
         <v>86</v>
       </c>
       <c r="N17" s="5"/>
@@ -4171,7 +4162,7 @@
       <c r="P17" s="5"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="71" t="s">
+      <c r="A18" s="66" t="s">
         <v>109</v>
       </c>
       <c r="B18" s="20">
@@ -4180,19 +4171,19 @@
       <c r="C18" s="20">
         <v>1</v>
       </c>
-      <c r="D18" s="62">
+      <c r="D18" s="58">
         <v>0.47</v>
       </c>
       <c r="E18" s="20">
         <v>12</v>
       </c>
-      <c r="F18" s="63">
+      <c r="F18" s="59">
         <v>60</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H18" s="55">
+      <c r="H18" s="53">
         <f t="shared" si="5"/>
         <v>0.47</v>
       </c>
@@ -4211,7 +4202,7 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="M18" s="64" t="s">
+      <c r="M18" s="60" t="s">
         <v>86</v>
       </c>
       <c r="N18" s="5"/>
@@ -4219,7 +4210,7 @@
       <c r="P18" s="5"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="71" t="s">
+      <c r="A19" s="66" t="s">
         <v>110</v>
       </c>
       <c r="B19" s="20">
@@ -4228,19 +4219,19 @@
       <c r="C19" s="20">
         <v>1</v>
       </c>
-      <c r="D19" s="62">
+      <c r="D19" s="58">
         <v>0.47</v>
       </c>
       <c r="E19" s="20">
         <v>12</v>
       </c>
-      <c r="F19" s="63">
+      <c r="F19" s="59">
         <v>60</v>
       </c>
       <c r="G19" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H19" s="55">
+      <c r="H19" s="53">
         <f t="shared" si="5"/>
         <v>0.47</v>
       </c>
@@ -4259,7 +4250,7 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="M19" s="64" t="s">
+      <c r="M19" s="60" t="s">
         <v>86</v>
       </c>
       <c r="N19" s="5"/>
@@ -4267,7 +4258,7 @@
       <c r="P19" s="5"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="72" t="s">
+      <c r="A20" s="67" t="s">
         <v>111</v>
       </c>
       <c r="B20" s="20">
@@ -4276,19 +4267,19 @@
       <c r="C20" s="20">
         <v>1</v>
       </c>
-      <c r="D20" s="62">
+      <c r="D20" s="58">
         <v>0.46</v>
       </c>
       <c r="E20" s="20">
         <v>5</v>
       </c>
-      <c r="F20" s="63">
+      <c r="F20" s="59">
         <v>60</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H20" s="55">
+      <c r="H20" s="53">
         <f t="shared" si="5"/>
         <v>0.46</v>
       </c>
@@ -4308,7 +4299,7 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="M20" s="64" t="s">
+      <c r="M20" s="60" t="s">
         <v>81</v>
       </c>
       <c r="N20" s="5"/>
@@ -4316,7 +4307,7 @@
       <c r="P20" s="5"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="72" t="s">
+      <c r="A21" s="67" t="s">
         <v>112</v>
       </c>
       <c r="B21" s="20">
@@ -4325,19 +4316,19 @@
       <c r="C21" s="20">
         <v>1</v>
       </c>
-      <c r="D21" s="62">
+      <c r="D21" s="58">
         <v>0.46</v>
       </c>
       <c r="E21" s="20">
         <v>5</v>
       </c>
-      <c r="F21" s="63">
+      <c r="F21" s="59">
         <v>60</v>
       </c>
       <c r="G21" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H21" s="55">
+      <c r="H21" s="53">
         <f t="shared" si="5"/>
         <v>0.46</v>
       </c>
@@ -4357,7 +4348,7 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="M21" s="64" t="s">
+      <c r="M21" s="60" t="s">
         <v>81</v>
       </c>
       <c r="N21" s="5"/>
@@ -4365,7 +4356,7 @@
       <c r="P21" s="5"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="72" t="s">
+      <c r="A22" s="67" t="s">
         <v>113</v>
       </c>
       <c r="B22" s="20">
@@ -4374,19 +4365,19 @@
       <c r="C22" s="20">
         <v>1</v>
       </c>
-      <c r="D22" s="62">
+      <c r="D22" s="58">
         <v>0.46</v>
       </c>
       <c r="E22" s="20">
         <v>5</v>
       </c>
-      <c r="F22" s="63">
+      <c r="F22" s="59">
         <v>60</v>
       </c>
       <c r="G22" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H22" s="55">
+      <c r="H22" s="53">
         <f t="shared" si="5"/>
         <v>0.46</v>
       </c>
@@ -4406,7 +4397,7 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="M22" s="64" t="s">
+      <c r="M22" s="60" t="s">
         <v>81</v>
       </c>
       <c r="N22" s="5"/>
@@ -4414,7 +4405,7 @@
       <c r="P22" s="5"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="66" t="s">
         <v>114</v>
       </c>
       <c r="B23" s="20">
@@ -4423,19 +4414,19 @@
       <c r="C23" s="20">
         <v>1</v>
       </c>
-      <c r="D23" s="62">
+      <c r="D23" s="58">
         <v>0.51</v>
       </c>
       <c r="E23" s="20">
         <v>5</v>
       </c>
-      <c r="F23" s="63">
+      <c r="F23" s="59">
         <v>60</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H23" s="55">
+      <c r="H23" s="53">
         <f t="shared" ref="H23" si="10">SUM(D23/C23)</f>
         <v>0.51</v>
       </c>
@@ -4455,7 +4446,7 @@
         <f t="shared" ref="L23" si="14">SUM(C23)</f>
         <v>1</v>
       </c>
-      <c r="M23" s="64" t="s">
+      <c r="M23" s="60" t="s">
         <v>85</v>
       </c>
       <c r="N23" s="5"/>
@@ -4463,7 +4454,7 @@
       <c r="P23" s="5"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="71" t="s">
+      <c r="A24" s="66" t="s">
         <v>115</v>
       </c>
       <c r="B24" s="20">
@@ -4472,19 +4463,19 @@
       <c r="C24" s="20">
         <v>1</v>
       </c>
-      <c r="D24" s="62">
+      <c r="D24" s="58">
         <v>0.51</v>
       </c>
       <c r="E24" s="20">
         <v>5</v>
       </c>
-      <c r="F24" s="63">
+      <c r="F24" s="59">
         <v>60</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H24" s="55">
+      <c r="H24" s="53">
         <f t="shared" ref="H24:H25" si="15">SUM(D24/C24)</f>
         <v>0.51</v>
       </c>
@@ -4504,7 +4495,7 @@
         <f t="shared" ref="L24:L25" si="19">SUM(C24)</f>
         <v>1</v>
       </c>
-      <c r="M24" s="64" t="s">
+      <c r="M24" s="60" t="s">
         <v>85</v>
       </c>
       <c r="N24" s="5"/>
@@ -4512,7 +4503,7 @@
       <c r="P24" s="5"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" s="71" t="s">
+      <c r="A25" s="66" t="s">
         <v>116</v>
       </c>
       <c r="B25" s="20">
@@ -4521,19 +4512,19 @@
       <c r="C25" s="20">
         <v>1</v>
       </c>
-      <c r="D25" s="62">
+      <c r="D25" s="58">
         <v>0.51</v>
       </c>
       <c r="E25" s="20">
         <v>5</v>
       </c>
-      <c r="F25" s="63">
+      <c r="F25" s="59">
         <v>60</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H25" s="55">
+      <c r="H25" s="53">
         <f t="shared" si="15"/>
         <v>0.51</v>
       </c>
@@ -4553,7 +4544,7 @@
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="M25" s="64" t="s">
+      <c r="M25" s="60" t="s">
         <v>85</v>
       </c>
       <c r="N25" s="5"/>
@@ -4561,7 +4552,7 @@
       <c r="P25" s="5"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" s="71" t="s">
+      <c r="A26" s="66" t="s">
         <v>117</v>
       </c>
       <c r="B26" s="20">
@@ -4570,19 +4561,19 @@
       <c r="C26" s="20">
         <v>1</v>
       </c>
-      <c r="D26" s="62">
+      <c r="D26" s="58">
         <v>1.0900000000000001</v>
       </c>
       <c r="E26" s="20">
         <v>12</v>
       </c>
-      <c r="F26" s="63">
+      <c r="F26" s="59">
         <v>64</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="H26" s="55">
+      <c r="H26" s="53">
         <f>SUM(D26/C26)</f>
         <v>1.0900000000000001</v>
       </c>
@@ -4602,7 +4593,7 @@
         <f>SUM(C26)</f>
         <v>1</v>
       </c>
-      <c r="M26" s="64" t="s">
+      <c r="M26" s="60" t="s">
         <v>87</v>
       </c>
       <c r="N26" s="5"/>
@@ -4610,7 +4601,7 @@
       <c r="P26" s="5"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" s="71" t="s">
+      <c r="A27" s="66" t="s">
         <v>118</v>
       </c>
       <c r="B27" s="20">
@@ -4619,19 +4610,19 @@
       <c r="C27" s="20">
         <v>1</v>
       </c>
-      <c r="D27" s="62">
+      <c r="D27" s="58">
         <v>1.19</v>
       </c>
       <c r="E27" s="20">
         <v>12</v>
       </c>
-      <c r="F27" s="63">
+      <c r="F27" s="59">
         <v>64</v>
       </c>
       <c r="G27" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="H27" s="55">
+      <c r="H27" s="53">
         <f>SUM(D27/C27)</f>
         <v>1.19</v>
       </c>
@@ -4651,7 +4642,7 @@
         <f>SUM(C27)</f>
         <v>1</v>
       </c>
-      <c r="M27" s="64" t="s">
+      <c r="M27" s="60" t="s">
         <v>88</v>
       </c>
       <c r="N27" s="5"/>
@@ -4659,946 +4650,946 @@
       <c r="P27" s="5"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" s="53" t="s">
+      <c r="A28" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="59" t="e">
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="53" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I28" s="60">
+      <c r="I28" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J28" s="60">
+      <c r="J28" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K28" s="60">
+      <c r="K28" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L28" s="60">
+      <c r="L28" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M28" s="42"/>
+      <c r="M28" s="40"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="53" t="s">
+      <c r="A29" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="59" t="e">
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="53" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I29" s="60">
+      <c r="I29" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J29" s="60">
+      <c r="J29" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K29" s="60">
+      <c r="K29" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L29" s="60">
+      <c r="L29" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M29" s="42"/>
+      <c r="M29" s="40"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A30" s="53" t="s">
+      <c r="A30" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="59" t="e">
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="53" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I30" s="60">
+      <c r="I30" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J30" s="60">
+      <c r="J30" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K30" s="60">
+      <c r="K30" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L30" s="60">
+      <c r="L30" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M30" s="42"/>
+      <c r="M30" s="40"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A31" s="53" t="s">
+      <c r="A31" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="59" t="e">
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="53" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I31" s="60">
+      <c r="I31" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J31" s="60">
+      <c r="J31" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K31" s="60">
+      <c r="K31" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L31" s="60">
+      <c r="L31" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M31" s="42"/>
+      <c r="M31" s="40"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A32" s="53" t="s">
+      <c r="A32" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="59" t="e">
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="53" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I32" s="60">
+      <c r="I32" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J32" s="60">
+      <c r="J32" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K32" s="60">
+      <c r="K32" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L32" s="60">
+      <c r="L32" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M32" s="42"/>
+      <c r="M32" s="40"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33" s="53" t="s">
+      <c r="A33" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="59" t="e">
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="53" t="e">
         <f t="shared" ref="H33:H54" si="20">SUM(D33/C33)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I33" s="60">
+      <c r="I33" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J33" s="60">
+      <c r="J33" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K33" s="60">
+      <c r="K33" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L33" s="60">
+      <c r="L33" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M33" s="42"/>
+      <c r="M33" s="40"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" s="53" t="s">
+      <c r="A34" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="59" t="e">
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I34" s="60">
+      <c r="I34" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J34" s="60">
+      <c r="J34" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K34" s="60">
+      <c r="K34" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L34" s="60">
+      <c r="L34" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M34" s="42"/>
+      <c r="M34" s="40"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A35" s="53" t="s">
+      <c r="A35" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="59" t="e">
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I35" s="60">
+      <c r="I35" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J35" s="60">
+      <c r="J35" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K35" s="60">
+      <c r="K35" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L35" s="60">
+      <c r="L35" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M35" s="42"/>
+      <c r="M35" s="40"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A36" s="53" t="s">
+      <c r="A36" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="59" t="e">
+      <c r="B36" s="41"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I36" s="60">
+      <c r="I36" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J36" s="60">
+      <c r="J36" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K36" s="60">
+      <c r="K36" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L36" s="60">
+      <c r="L36" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M36" s="42"/>
+      <c r="M36" s="40"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A37" s="53" t="s">
+      <c r="A37" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="59" t="e">
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I37" s="60">
+      <c r="I37" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J37" s="60">
+      <c r="J37" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K37" s="60">
+      <c r="K37" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L37" s="60">
+      <c r="L37" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M37" s="42"/>
+      <c r="M37" s="40"/>
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A38" s="53" t="s">
+      <c r="A38" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="59" t="e">
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I38" s="60">
+      <c r="I38" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J38" s="60">
+      <c r="J38" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K38" s="60">
+      <c r="K38" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L38" s="60">
+      <c r="L38" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M38" s="42"/>
+      <c r="M38" s="40"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A39" s="53" t="s">
+      <c r="A39" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B39" s="43"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="54"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="59" t="e">
+      <c r="B39" s="41"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="52"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I39" s="60">
+      <c r="I39" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J39" s="60">
+      <c r="J39" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K39" s="60">
+      <c r="K39" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L39" s="60">
+      <c r="L39" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M39" s="42"/>
+      <c r="M39" s="40"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A40" s="53" t="s">
+      <c r="A40" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B40" s="43"/>
-      <c r="C40" s="43"/>
-      <c r="D40" s="54"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
-      <c r="H40" s="59" t="e">
+      <c r="B40" s="41"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="52"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="41"/>
+      <c r="G40" s="41"/>
+      <c r="H40" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I40" s="60">
+      <c r="I40" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J40" s="60">
+      <c r="J40" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K40" s="60">
+      <c r="K40" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L40" s="60">
+      <c r="L40" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M40" s="42"/>
+      <c r="M40" s="40"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A41" s="53" t="s">
+      <c r="A41" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="43"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="59" t="e">
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="41"/>
+      <c r="F41" s="41"/>
+      <c r="G41" s="41"/>
+      <c r="H41" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I41" s="60">
+      <c r="I41" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J41" s="60">
+      <c r="J41" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K41" s="60">
+      <c r="K41" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L41" s="60">
+      <c r="L41" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M41" s="42"/>
+      <c r="M41" s="40"/>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
       <c r="P41" s="5"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A42" s="53" t="s">
+      <c r="A42" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B42" s="43"/>
-      <c r="C42" s="43"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="43"/>
-      <c r="H42" s="59" t="e">
+      <c r="B42" s="41"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="41"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I42" s="60">
+      <c r="I42" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J42" s="60">
+      <c r="J42" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K42" s="60">
+      <c r="K42" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L42" s="60">
+      <c r="L42" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M42" s="42"/>
+      <c r="M42" s="40"/>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
       <c r="P42" s="5"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A43" s="53" t="s">
+      <c r="A43" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="43"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="59" t="e">
+      <c r="B43" s="41"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="52"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="41"/>
+      <c r="H43" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I43" s="60">
+      <c r="I43" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J43" s="60">
+      <c r="J43" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K43" s="60">
+      <c r="K43" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L43" s="60">
+      <c r="L43" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M43" s="42"/>
+      <c r="M43" s="40"/>
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
       <c r="P43" s="5"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A44" s="53" t="s">
+      <c r="A44" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="43"/>
-      <c r="C44" s="43"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="59" t="e">
+      <c r="B44" s="41"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="41"/>
+      <c r="G44" s="41"/>
+      <c r="H44" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I44" s="60">
+      <c r="I44" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J44" s="60">
+      <c r="J44" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K44" s="60">
+      <c r="K44" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L44" s="60">
+      <c r="L44" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M44" s="42"/>
+      <c r="M44" s="40"/>
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
       <c r="P44" s="5"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A45" s="53" t="s">
+      <c r="A45" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="43"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="54"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="59" t="e">
+      <c r="B45" s="41"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="41"/>
+      <c r="F45" s="41"/>
+      <c r="G45" s="41"/>
+      <c r="H45" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I45" s="60">
+      <c r="I45" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J45" s="60">
+      <c r="J45" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K45" s="60">
+      <c r="K45" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L45" s="60">
+      <c r="L45" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M45" s="42"/>
+      <c r="M45" s="40"/>
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
       <c r="P45" s="5"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A46" s="53" t="s">
+      <c r="A46" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
-      <c r="H46" s="59" t="e">
+      <c r="B46" s="41"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="41"/>
+      <c r="H46" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I46" s="60">
+      <c r="I46" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J46" s="60">
+      <c r="J46" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K46" s="60">
+      <c r="K46" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L46" s="60">
+      <c r="L46" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M46" s="42"/>
+      <c r="M46" s="40"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
       <c r="P46" s="5"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A47" s="53" t="s">
+      <c r="A47" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="43"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="54"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="59" t="e">
+      <c r="B47" s="41"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="52"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I47" s="60">
+      <c r="I47" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J47" s="60">
+      <c r="J47" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K47" s="60">
+      <c r="K47" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L47" s="60">
+      <c r="L47" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M47" s="42"/>
+      <c r="M47" s="40"/>
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A48" s="53" t="s">
+      <c r="A48" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B48" s="43"/>
-      <c r="C48" s="43"/>
-      <c r="D48" s="54"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="59" t="e">
+      <c r="B48" s="41"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="41"/>
+      <c r="G48" s="41"/>
+      <c r="H48" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I48" s="60">
+      <c r="I48" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J48" s="60">
+      <c r="J48" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K48" s="60">
+      <c r="K48" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L48" s="60">
+      <c r="L48" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M48" s="42"/>
+      <c r="M48" s="40"/>
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
       <c r="P48" s="5"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A49" s="53" t="s">
+      <c r="A49" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="43"/>
-      <c r="C49" s="43"/>
-      <c r="D49" s="54"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="43"/>
-      <c r="H49" s="59" t="e">
+      <c r="B49" s="41"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="52"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="41"/>
+      <c r="H49" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I49" s="60">
+      <c r="I49" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J49" s="60">
+      <c r="J49" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K49" s="60">
+      <c r="K49" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L49" s="60">
+      <c r="L49" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M49" s="42"/>
+      <c r="M49" s="40"/>
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
       <c r="P49" s="5"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A50" s="53" t="s">
+      <c r="A50" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="43"/>
-      <c r="C50" s="43"/>
-      <c r="D50" s="54"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="59" t="e">
+      <c r="B50" s="41"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="52"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="41"/>
+      <c r="H50" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I50" s="60">
+      <c r="I50" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J50" s="60">
+      <c r="J50" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K50" s="60">
+      <c r="K50" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L50" s="60">
+      <c r="L50" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M50" s="42"/>
+      <c r="M50" s="40"/>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A51" s="53" t="s">
+      <c r="A51" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="43"/>
-      <c r="C51" s="43"/>
-      <c r="D51" s="54"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="43"/>
-      <c r="H51" s="59" t="e">
+      <c r="B51" s="41"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="52"/>
+      <c r="E51" s="41"/>
+      <c r="F51" s="41"/>
+      <c r="G51" s="41"/>
+      <c r="H51" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I51" s="60">
+      <c r="I51" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J51" s="60">
+      <c r="J51" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K51" s="60">
+      <c r="K51" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L51" s="60">
+      <c r="L51" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M51" s="42"/>
+      <c r="M51" s="40"/>
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
       <c r="P51" s="5"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A52" s="53" t="s">
+      <c r="A52" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="43"/>
-      <c r="C52" s="43"/>
-      <c r="D52" s="54"/>
-      <c r="E52" s="43"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="43"/>
-      <c r="H52" s="59" t="e">
+      <c r="B52" s="41"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="52"/>
+      <c r="E52" s="41"/>
+      <c r="F52" s="41"/>
+      <c r="G52" s="41"/>
+      <c r="H52" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I52" s="60">
+      <c r="I52" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J52" s="60">
+      <c r="J52" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K52" s="60">
+      <c r="K52" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L52" s="60">
+      <c r="L52" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M52" s="42"/>
+      <c r="M52" s="40"/>
       <c r="N52" s="5"/>
       <c r="O52" s="5"/>
       <c r="P52" s="5"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A53" s="53" t="s">
+      <c r="A53" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="43"/>
-      <c r="C53" s="43"/>
-      <c r="D53" s="54"/>
-      <c r="E53" s="43"/>
-      <c r="F53" s="43"/>
-      <c r="G53" s="43"/>
-      <c r="H53" s="59" t="e">
+      <c r="B53" s="41"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="52"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="41"/>
+      <c r="H53" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I53" s="60">
+      <c r="I53" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J53" s="60">
+      <c r="J53" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K53" s="60">
+      <c r="K53" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L53" s="60">
+      <c r="L53" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M53" s="42"/>
+      <c r="M53" s="40"/>
       <c r="N53" s="5"/>
       <c r="O53" s="5"/>
       <c r="P53" s="5"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A54" s="53" t="s">
+      <c r="A54" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B54" s="43"/>
-      <c r="C54" s="43"/>
-      <c r="D54" s="54"/>
-      <c r="E54" s="43"/>
-      <c r="F54" s="43"/>
-      <c r="G54" s="43"/>
-      <c r="H54" s="59" t="e">
+      <c r="B54" s="41"/>
+      <c r="C54" s="41"/>
+      <c r="D54" s="52"/>
+      <c r="E54" s="41"/>
+      <c r="F54" s="41"/>
+      <c r="G54" s="41"/>
+      <c r="H54" s="53" t="e">
         <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I54" s="60">
+      <c r="I54" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J54" s="60">
+      <c r="J54" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K54" s="60">
+      <c r="K54" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L54" s="60">
+      <c r="L54" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M54" s="42"/>
+      <c r="M54" s="40"/>
       <c r="N54" s="5"/>
       <c r="O54" s="5"/>
       <c r="P54" s="5"/>
@@ -5644,38 +5635,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="93"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="87"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">

</xml_diff>